<commit_message>
Created scripts: sign in to ebay app search a product and verify the details
</commit_message>
<xml_diff>
--- a/EbayAutomation/src/test/resources/datasheet.xlsx
+++ b/EbayAutomation/src/test/resources/datasheet.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Appium_Automation\Git\EbayAutomation\src\test\resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Appium_Automation\Git\Automation\EbayAutomation\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="12765" windowHeight="5520"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="12765" windowHeight="5520" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="sign_in" sheetId="1" r:id="rId1"/>
@@ -48,10 +48,10 @@
     <t>Pandu@009</t>
   </si>
   <si>
-    <t>samsung TV</t>
-  </si>
-  <si>
     <t>pandurangan.gk@gmail.com</t>
+  </si>
+  <si>
+    <t>65-inch TV</t>
   </si>
 </sst>
 </file>
@@ -483,7 +483,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
@@ -513,7 +513,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C2" s="6" t="s">
         <v>6</v>
@@ -533,7 +533,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -549,7 +549,7 @@
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>